<commit_message>
update test view point login, register
</commit_message>
<xml_diff>
--- a/WIP/Users/LucPT/FAP_TestViewpoint_Login_v1.0_EN.xlsx
+++ b/WIP/Users/LucPT/FAP_TestViewpoint_Login_v1.0_EN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -3116,6 +3116,27 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3133,27 +3154,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="30" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3555,20 +3555,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>667897</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152857</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>391058</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57828</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3587,8 +3587,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1362075" y="666750"/>
-          <a:ext cx="8221222" cy="3277057"/>
+          <a:off x="2057400" y="533400"/>
+          <a:ext cx="3820058" cy="4858428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6303,14 +6303,14 @@
     <row r="2" spans="1:8" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="110"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="104"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="B3" s="6"/>
@@ -6325,12 +6325,12 @@
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="111" t="s">
+      <c r="C4" s="105" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
       <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
@@ -6342,27 +6342,27 @@
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="C6" s="107" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="12" t="s">
         <v>6</v>
       </c>
@@ -6371,11 +6371,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" customHeight="1">
-      <c r="B7" s="112"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
       <c r="G7" s="12" t="s">
         <v>7</v>
       </c>
@@ -6398,10 +6398,10 @@
       <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="107" t="s">
+      <c r="C9" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="108"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="19" t="s">
         <v>11</v>
       </c>
@@ -6419,10 +6419,10 @@
       <c r="B10" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="104"/>
+      <c r="D10" s="111"/>
       <c r="E10" s="23" t="s">
         <v>15</v>
       </c>
@@ -6436,8 +6436,8 @@
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" ht="13.5" customHeight="1">
       <c r="B11" s="27"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="104"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="23"/>
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
@@ -6445,8 +6445,8 @@
     </row>
     <row r="12" spans="1:8" s="21" customFormat="1">
       <c r="B12" s="29"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="113"/>
       <c r="E12" s="30"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
@@ -6454,8 +6454,8 @@
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1">
       <c r="B13" s="29"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="104"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="30"/>
       <c r="F13" s="24"/>
       <c r="G13" s="31"/>
@@ -6463,8 +6463,8 @@
     </row>
     <row r="14" spans="1:8" s="21" customFormat="1">
       <c r="B14" s="29"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="104"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="30"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -6472,8 +6472,8 @@
     </row>
     <row r="15" spans="1:8" s="21" customFormat="1">
       <c r="B15" s="29"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="104"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="30"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
@@ -6481,8 +6481,8 @@
     </row>
     <row r="16" spans="1:8" ht="13.5" thickBot="1">
       <c r="B16" s="32"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="109"/>
       <c r="E16" s="33"/>
       <c r="F16" s="34"/>
       <c r="G16" s="35"/>
@@ -6490,12 +6490,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -6503,6 +6497,12 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
   </mergeCells>
   <pageMargins left="0.47013888888888888" right="0.47013888888888888" top="0.5" bottom="0.35138888888888886" header="0.51180555555555562" footer="0.1701388888888889"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6518,7 +6518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -8208,8 +8208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>